<commit_message>
duplication error message check
</commit_message>
<xml_diff>
--- a/OBTBS_Automation/test.xlsx
+++ b/OBTBS_Automation/test.xlsx
@@ -22,22 +22,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t xml:space="preserve">ca</t>
+    <t xml:space="preserve">MG</t>
   </si>
   <si>
-    <t xml:space="preserve">name one</t>
+    <t xml:space="preserve">Meghalaya</t>
   </si>
   <si>
-    <t xml:space="preserve">cb</t>
+    <t xml:space="preserve">BR</t>
   </si>
   <si>
-    <t xml:space="preserve">name two</t>
+    <t xml:space="preserve">West Bengal</t>
   </si>
   <si>
-    <t xml:space="preserve">cc</t>
+    <t xml:space="preserve">UK</t>
   </si>
   <si>
-    <t xml:space="preserve">name three</t>
+    <t xml:space="preserve">Utharakhand</t>
   </si>
 </sst>
 </file>
@@ -141,10 +141,15 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>